<commit_message>
added paragon to excel doc
</commit_message>
<xml_diff>
--- a/noble positions update.xlsx
+++ b/noble positions update.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fbfshare\RedirectedFolders\rbrown\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbrown\Dropbox\DF_mods\Nobles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="55">
   <si>
     <t>Position</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>This chart was taken from Dwarf Fortress wiki, but updated to match the changes in the mod.</t>
+  </si>
+  <si>
+    <t>Paragon</t>
+  </si>
+  <si>
+    <t>Optional</t>
   </si>
 </sst>
 </file>
@@ -226,13 +232,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,6 +1325,46 @@
         <v>16</v>
       </c>
     </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A4:K23">
     <sortCondition ref="A4:A23"/>

</xml_diff>